<commit_message>
More client requested fixes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/education_yr12_2015_uploader/education_yr12_2015.xlsx
+++ b/dashboard_loader/education_yr12_2015_uploader/education_yr12_2015.xlsx
@@ -113,7 +113,7 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">ABS Survey of Education and Work, various years and ABS 2006 and 2011 Census.</t>
+    <t xml:space="preserve">ABS Survey of Education and Work, various years and ABS 2006 and 2011 Census of Population and Housing..</t>
   </si>
 </sst>
 </file>
@@ -125,7 +125,7 @@
     <numFmt numFmtId="165" formatCode="########\ ###\ ##0.0;\-########\ ###\ ##0.0;\–"/>
     <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -147,87 +147,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -257,7 +176,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,74 +185,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF00000A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -351,7 +213,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -375,156 +237,100 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="2" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="3" xfId="36" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="36" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="36" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF00000A"/>
-      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -536,7 +342,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -552,7 +358,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -582,7 +388,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L19" activeCellId="0" sqref="L19"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="B9 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -635,30 +441,30 @@
         <v>11</v>
       </c>
       <c r="C2" s="4" t="n">
-        <v>81.9</v>
+        <v>82.8157993434066</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>85.4</v>
+        <v>86.1068933613156</v>
       </c>
       <c r="E2" s="4" t="n">
-        <v>82.2</v>
+        <v>83.1261392262478</v>
       </c>
       <c r="F2" s="4" t="n">
-        <v>79.3</v>
+        <v>80.3243278624143</v>
       </c>
       <c r="G2" s="4" t="n">
-        <v>76.4</v>
+        <v>77.7768168895327</v>
       </c>
       <c r="H2" s="4" t="n">
-        <v>72.9</v>
+        <v>74.5882617158257</v>
       </c>
       <c r="I2" s="4" t="n">
-        <v>90.2</v>
+        <v>90.5751232961827</v>
       </c>
       <c r="J2" s="4" t="n">
-        <v>56.5</v>
-      </c>
-      <c r="K2" s="4" t="n">
+        <v>58.1665077851922</v>
+      </c>
+      <c r="K2" s="5" t="n">
         <v>82.8</v>
       </c>
     </row>
@@ -840,15 +646,15 @@
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5" t="n">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="n">
         <v>85.6</v>
       </c>
     </row>
@@ -859,15 +665,15 @@
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5" t="n">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -878,15 +684,15 @@
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5" t="n">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="n">
         <v>0.759345794392523</v>
       </c>
     </row>
@@ -897,31 +703,31 @@
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="6" t="n">
-        <v>84.1</v>
-      </c>
-      <c r="D15" s="6" t="n">
-        <v>87.4</v>
-      </c>
-      <c r="E15" s="6" t="n">
-        <v>83.9</v>
-      </c>
-      <c r="F15" s="6" t="n">
-        <v>82.2</v>
-      </c>
-      <c r="G15" s="6" t="n">
-        <v>80.6</v>
-      </c>
-      <c r="H15" s="6" t="n">
-        <v>75.6</v>
-      </c>
-      <c r="I15" s="6" t="n">
-        <v>90.6</v>
-      </c>
-      <c r="J15" s="6" t="n">
-        <v>63.1</v>
-      </c>
-      <c r="K15" s="6" t="n">
+      <c r="C15" s="7" t="n">
+        <v>84.8</v>
+      </c>
+      <c r="D15" s="7" t="n">
+        <v>88</v>
+      </c>
+      <c r="E15" s="7" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="F15" s="7" t="n">
+        <v>83.1</v>
+      </c>
+      <c r="G15" s="7" t="n">
+        <v>81.8</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <v>77.2</v>
+      </c>
+      <c r="I15" s="7" t="n">
+        <v>91</v>
+      </c>
+      <c r="J15" s="7" t="n">
+        <v>64.4</v>
+      </c>
+      <c r="K15" s="8" t="n">
         <v>84.1</v>
       </c>
     </row>
@@ -932,15 +738,15 @@
       <c r="B16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5" t="n">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -951,15 +757,15 @@
       <c r="B17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5" t="n">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6" t="n">
         <v>0.772889417360285</v>
       </c>
     </row>
@@ -970,15 +776,15 @@
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5" t="n">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6" t="n">
         <v>85.9</v>
       </c>
     </row>
@@ -989,15 +795,15 @@
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5" t="n">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6" t="n">
         <v>1.3</v>
       </c>
     </row>
@@ -1008,15 +814,15 @@
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5" t="n">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6" t="n">
         <v>0.756693830034924</v>
       </c>
     </row>
@@ -1027,15 +833,15 @@
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5" t="n">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6" t="n">
         <v>86.7</v>
       </c>
     </row>
@@ -1046,15 +852,15 @@
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5" t="n">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6" t="n">
         <v>1.5</v>
       </c>
     </row>
@@ -1065,15 +871,15 @@
       <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5" t="n">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6" t="n">
         <v>0.865051903114187</v>
       </c>
     </row>
@@ -1084,15 +890,15 @@
       <c r="B24" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5" t="n">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6" t="n">
         <v>86.1</v>
       </c>
     </row>
@@ -1103,15 +909,15 @@
       <c r="B25" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5" t="n">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6" t="n">
         <v>1.5</v>
       </c>
     </row>
@@ -1122,15 +928,15 @@
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5" t="n">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6" t="n">
         <v>0.871080139372822</v>
       </c>
     </row>
@@ -1141,15 +947,15 @@
       <c r="B27" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5" t="n">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6" t="n">
         <v>88.4</v>
       </c>
     </row>
@@ -1160,15 +966,15 @@
       <c r="B28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5" t="n">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6" t="n">
         <v>1.1</v>
       </c>
     </row>
@@ -1179,34 +985,34 @@
       <c r="B29" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5" t="n">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6" t="n">
         <v>0.622171945701358</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="n">
         <v>2015</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5" t="n">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6" t="n">
         <v>90</v>
       </c>
     </row>
@@ -1229,79 +1035,79 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="7" width="67.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="7" width="9.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="9" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="9" width="67.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="9" width="9.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="14" t="n">
         <v>2015</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="15" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="49.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="1" t="s">

</xml_diff>